<commit_message>
- poprawa błędu Radom->Rzeszów
</commit_message>
<xml_diff>
--- a/wynagrodzenia_pl_2024.xlsx
+++ b/wynagrodzenia_pl_2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studia AG II\Semestr 1\Analiza danych\Analiza_Danych_Projekt_1\Cenowe_Rozkminy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE4D2B4-CC1D-4AF9-9D89-B1734E161E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54EBC274-7638-4163-A256-3FBCE9B816DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OPIS" sheetId="1" r:id="rId1"/>
@@ -207,10 +207,10 @@
     <t>Częstochowa</t>
   </si>
   <si>
-    <t>Radom</t>
-  </si>
-  <si>
     <t>Białystok</t>
+  </si>
+  <si>
+    <t>Rzeszów</t>
   </si>
 </sst>
 </file>
@@ -291,11 +291,11 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Kolumna" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -693,7 +693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
@@ -703,10 +703,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -714,22 +714,22 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
       <c r="C2" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
       <c r="C3" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
       <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
@@ -934,8 +934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A277956-7A3C-4AEB-9EE4-0FA8075B4816}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,10 +945,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>57</v>
       </c>
     </row>
@@ -961,7 +961,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>58</v>
       </c>
       <c r="B3">
@@ -969,15 +969,15 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>10173.41</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>60</v>
       </c>
       <c r="B5">
@@ -985,16 +985,16 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="6">
+        <v>7187.74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="B6" s="7">
-        <v>7368</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>62</v>
       </c>
       <c r="B7">
         <v>6806.05</v>

</xml_diff>

<commit_message>
- poprawa analizowanego miasta z Gdańska na Radom
</commit_message>
<xml_diff>
--- a/wynagrodzenia_pl_2024.xlsx
+++ b/wynagrodzenia_pl_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studia AG II\Semestr 1\Analiza danych\Analiza_Danych_Projekt_1\Cenowe_Rozkminy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54EBC274-7638-4163-A256-3FBCE9B816DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80EFBCB0-AD30-4F75-8591-0DE5407CC176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -192,9 +192,6 @@
     <t>Miasto</t>
   </si>
   <si>
-    <t>Gdańsk </t>
-  </si>
-  <si>
     <t>Wynagrodzenie</t>
   </si>
   <si>
@@ -211,6 +208,9 @@
   </si>
   <si>
     <t>Rzeszów</t>
+  </si>
+  <si>
+    <t>Radom</t>
   </si>
 </sst>
 </file>
@@ -932,10 +932,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A277956-7A3C-4AEB-9EE4-0FA8075B4816}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -949,20 +949,20 @@
         <v>55</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>56</v>
+      <c r="A2" s="5" t="s">
+        <v>62</v>
       </c>
       <c r="B2">
-        <v>10017.25</v>
+        <v>7368</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3">
         <v>9673.42</v>
@@ -970,7 +970,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="5">
         <v>10173.41</v>
@@ -978,7 +978,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5">
         <v>8380.2800000000007</v>
@@ -986,7 +986,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" s="6">
         <v>7187.74</v>
@@ -994,11 +994,14 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7">
         <v>6806.05</v>
       </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>